<commit_message>
Update FTICRMS SPE dilutions template_filled_out AMP.xlsx
</commit_message>
<xml_diff>
--- a/SPE/FTICRMS SPE dilutions template_filled_out AMP.xlsx
+++ b/SPE/FTICRMS SPE dilutions template_filled_out AMP.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/myer056/GitHub/tempest_ionic_strength/SPE/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78851FF5-9FB7-EC42-BD9F-E9594679DB3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9276BA1F-4D29-1046-8BD8-AB9A4B5A6263}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2460" yWindow="760" windowWidth="29460" windowHeight="19580" activeTab="2" xr2:uid="{88C78EEA-1365-A44C-9080-7B0F676A2065}"/>
+    <workbookView xWindow="2460" yWindow="760" windowWidth="29460" windowHeight="19580" xr2:uid="{88C78EEA-1365-A44C-9080-7B0F676A2065}"/>
   </bookViews>
   <sheets>
     <sheet name="dilutions_calculations_sheet" sheetId="1" r:id="rId1"/>
@@ -56,6 +56,13 @@
     <author>tc={37DA5A24-29F1-E242-9556-9DD6F3843AA1}</author>
     <author>tc={9C8F4C2F-1FC4-334F-B176-2C57EE89F90D}</author>
     <author>tc={8A8F13C9-8DCE-A949-8425-68EC367E9F76}</author>
+    <author>tc={9A01890A-4B2F-E647-BEDB-253AB5292843}</author>
+    <author>tc={192DB8F0-C8DE-4949-8EFA-4BC6E535851A}</author>
+    <author>tc={34729BAC-AA39-8F4D-9B3C-F2B8469140A5}</author>
+    <author>tc={9738570D-41F4-B647-B361-DB2D65F10557}</author>
+    <author>tc={A881E988-A5A1-764B-928C-B041308BD189}</author>
+    <author>tc={5607CF95-9E9A-E941-935C-F528320DA1A8}</author>
+    <author>tc={583C19B6-1B5F-4C40-ACCC-552EA1EA4249}</author>
   </authors>
   <commentList>
     <comment ref="C1" authorId="0" shapeId="0" xr:uid="{68620E2D-7D45-41C0-A72B-F4AB141BC9A7}">
@@ -188,6 +195,62 @@
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Actual concentration of diluted FTICRMS sample assuming 60% extraction efficiency.</t>
+      </text>
+    </comment>
+    <comment ref="A117" authorId="16" shapeId="0" xr:uid="{9A01890A-4B2F-E647-BEDB-253AB5292843}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Not sure they were actually eluted. Volumes are a guess based on the other samples</t>
+      </text>
+    </comment>
+    <comment ref="A118" authorId="17" shapeId="0" xr:uid="{192DB8F0-C8DE-4949-8EFA-4BC6E535851A}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Not sure they were actually eluted. Volumes are a guess based on the other samples</t>
+      </text>
+    </comment>
+    <comment ref="A119" authorId="18" shapeId="0" xr:uid="{34729BAC-AA39-8F4D-9B3C-F2B8469140A5}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Not sure they were actually eluted. Volumes are a guess based on the other samples</t>
+      </text>
+    </comment>
+    <comment ref="A120" authorId="19" shapeId="0" xr:uid="{9738570D-41F4-B647-B361-DB2D65F10557}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Not sure they were actually eluted. Volumes are a guess based on the other samples</t>
+      </text>
+    </comment>
+    <comment ref="A121" authorId="20" shapeId="0" xr:uid="{A881E988-A5A1-764B-928C-B041308BD189}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Not sure they were actually eluted. Volumes are a guess based on the other samples</t>
+      </text>
+    </comment>
+    <comment ref="A122" authorId="21" shapeId="0" xr:uid="{5607CF95-9E9A-E941-935C-F528320DA1A8}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Not sure they were actually eluted. Volumes are a guess based on the other samples</t>
+      </text>
+    </comment>
+    <comment ref="A123" authorId="22" shapeId="0" xr:uid="{583C19B6-1B5F-4C40-ACCC-552EA1EA4249}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Not sure they were actually eluted. Volumes are a guess based on the other samples</t>
       </text>
     </comment>
   </commentList>
@@ -659,7 +722,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="372">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="379">
   <si>
     <t>Sample_ID</t>
   </si>
@@ -1775,6 +1838,27 @@
   </si>
   <si>
     <t>EUP60985_41</t>
+  </si>
+  <si>
+    <t>TMP_0.B.2_EXP</t>
+  </si>
+  <si>
+    <t>TMP_0.C.2_EXP</t>
+  </si>
+  <si>
+    <t>TMP_1.A.1_EXP</t>
+  </si>
+  <si>
+    <t>TMP_25.B.1_EXP</t>
+  </si>
+  <si>
+    <t>TMP_25.C.2_EXP</t>
+  </si>
+  <si>
+    <t>TMP_25.C.6_EXP</t>
+  </si>
+  <si>
+    <t>TMP_25.C.4_EXP</t>
   </si>
 </sst>
 </file>
@@ -2020,7 +2104,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2131,6 +2215,23 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2507,6 +2608,27 @@
   <threadedComment ref="W1" dT="2022-10-14T20:08:47.20" personId="{42B7E531-F973-4941-A3F1-2E0A918A88E7}" id="{8A8F13C9-8DCE-A949-8425-68EC367E9F76}">
     <text>Actual concentration of diluted FTICRMS sample assuming 60% extraction efficiency.</text>
   </threadedComment>
+  <threadedComment ref="A117" dT="2024-04-04T16:25:23.84" personId="{C9156CD5-0306-403E-86D7-3E19D63E8616}" id="{9A01890A-4B2F-E647-BEDB-253AB5292843}">
+    <text>Not sure they were actually eluted. Volumes are a guess based on the other samples</text>
+  </threadedComment>
+  <threadedComment ref="A118" dT="2024-04-04T16:25:23.84" personId="{C9156CD5-0306-403E-86D7-3E19D63E8616}" id="{192DB8F0-C8DE-4949-8EFA-4BC6E535851A}">
+    <text>Not sure they were actually eluted. Volumes are a guess based on the other samples</text>
+  </threadedComment>
+  <threadedComment ref="A119" dT="2024-04-04T16:25:23.84" personId="{C9156CD5-0306-403E-86D7-3E19D63E8616}" id="{34729BAC-AA39-8F4D-9B3C-F2B8469140A5}">
+    <text>Not sure they were actually eluted. Volumes are a guess based on the other samples</text>
+  </threadedComment>
+  <threadedComment ref="A120" dT="2024-04-04T16:25:23.84" personId="{C9156CD5-0306-403E-86D7-3E19D63E8616}" id="{9738570D-41F4-B647-B361-DB2D65F10557}">
+    <text>Not sure they were actually eluted. Volumes are a guess based on the other samples</text>
+  </threadedComment>
+  <threadedComment ref="A121" dT="2024-04-04T16:25:23.84" personId="{C9156CD5-0306-403E-86D7-3E19D63E8616}" id="{A881E988-A5A1-764B-928C-B041308BD189}">
+    <text>Not sure they were actually eluted. Volumes are a guess based on the other samples</text>
+  </threadedComment>
+  <threadedComment ref="A122" dT="2024-04-04T16:25:23.84" personId="{C9156CD5-0306-403E-86D7-3E19D63E8616}" id="{5607CF95-9E9A-E941-935C-F528320DA1A8}">
+    <text>Not sure they were actually eluted. Volumes are a guess based on the other samples</text>
+  </threadedComment>
+  <threadedComment ref="A123" dT="2024-04-04T16:25:23.84" personId="{C9156CD5-0306-403E-86D7-3E19D63E8616}" id="{583C19B6-1B5F-4C40-ACCC-552EA1EA4249}">
+    <text>Not sure they were actually eluted. Volumes are a guess based on the other samples</text>
+  </threadedComment>
 </ThreadedComments>
 </file>
 
@@ -2689,8 +2811,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7D07A3E-9050-4F42-8C8E-5CEE8C3DD998}">
   <dimension ref="A1:X207"/>
   <sheetViews>
-    <sheetView zoomScale="89" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="O99" sqref="O99"/>
+    <sheetView tabSelected="1" topLeftCell="I79" zoomScale="89" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="P124" sqref="P124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2862,15 +2984,15 @@
         <v>0</v>
       </c>
       <c r="U2">
-        <f t="shared" ref="U2:U33" si="6">(S2/0.792)*1000</f>
+        <f t="shared" ref="U2:U3" si="6">(S2/0.792)*1000</f>
         <v>0</v>
       </c>
       <c r="V2">
-        <f t="shared" ref="V2:V33" si="7">(T2/0.792)*1000</f>
+        <f t="shared" ref="V2:V3" si="7">(T2/0.792)*1000</f>
         <v>0</v>
       </c>
       <c r="W2" s="18" t="e">
-        <f t="shared" ref="W2:W33" si="8">((U2*I2)/(U2+V2))</f>
+        <f t="shared" ref="W2:W3" si="8">((U2*I2)/(U2+V2))</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -2932,11 +3054,11 @@
         <v>13.928135356706775</v>
       </c>
       <c r="Q3" s="15">
-        <f t="shared" ref="Q3:Q67" si="9">O3*0.7921/1000</f>
+        <f t="shared" ref="Q3" si="9">O3*0.7921/1000</f>
         <v>0.34541252398395256</v>
       </c>
       <c r="R3" s="15">
-        <f t="shared" ref="R3:R67" si="10">P3*0.7921</f>
+        <f t="shared" ref="R3" si="10">P3*0.7921</f>
         <v>11.032476016047438</v>
       </c>
       <c r="S3">
@@ -3010,7 +3132,7 @@
         <v>0.45</v>
       </c>
       <c r="O4" s="4">
-        <f t="shared" ref="O4:O67" si="11">(M4*N4)*1000/J4</f>
+        <f t="shared" ref="O4:O66" si="11">(M4*N4)*1000/J4</f>
         <v>441.6961130742049</v>
       </c>
       <c r="P4" s="4">
@@ -8493,7 +8615,7 @@
         <v>0.45</v>
       </c>
       <c r="O68" s="4">
-        <f t="shared" ref="O68:O116" si="35">(M68*N68)*1000/J68</f>
+        <f t="shared" ref="O68:O97" si="35">(M68*N68)*1000/J68</f>
         <v>310.17369727047145</v>
       </c>
       <c r="P68" s="4">
@@ -11108,31 +11230,34 @@
       <c r="B99" t="s">
         <v>352</v>
       </c>
+      <c r="C99">
+        <v>0</v>
+      </c>
       <c r="F99" s="3">
-        <f t="shared" ref="F99:F116" si="42">C99*D99/1000</f>
+        <f t="shared" ref="F99:F117" si="42">C99*D99/1000</f>
         <v>0</v>
       </c>
       <c r="G99" s="3">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H99" s="3" t="e">
-        <f t="shared" ref="H99:H116" si="43">1/(F99/G99)</f>
+        <f t="shared" ref="H99:H117" si="43">1/(F99/G99)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="I99" s="3" t="e">
-        <f t="shared" ref="I99:I116" si="44">(C99*D99/E99)*0.6</f>
+        <f t="shared" ref="I99:I117" si="44">(C99*D99/E99)*0.6</f>
         <v>#DIV/0!</v>
       </c>
       <c r="J99" s="3" t="e">
-        <f t="shared" ref="J99:J116" si="45">(C99*D99/E99)*0.45</f>
+        <f t="shared" ref="J99:J117" si="45">(C99*D99/E99)*0.45</f>
         <v>#DIV/0!</v>
       </c>
       <c r="K99" s="35" t="e">
-        <f t="shared" ref="K99:K116" si="46">(C99*D99/E99)</f>
+        <f t="shared" ref="K99:K117" si="46">(C99*D99/E99)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="L99" t="e">
-        <f t="shared" ref="L99:L116" si="47">J99*E99/1000</f>
+        <f t="shared" ref="L99:L117" si="47">J99*E99/1000</f>
         <v>#DIV/0!</v>
       </c>
       <c r="M99" s="5">
@@ -11184,12 +11309,15 @@
       <c r="B100" t="s">
         <v>353</v>
       </c>
+      <c r="C100">
+        <v>0</v>
+      </c>
       <c r="F100" s="3">
         <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="G100" s="3">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="H100" s="3" t="e">
         <f t="shared" si="43"/>
@@ -11260,12 +11388,15 @@
       <c r="B101" t="s">
         <v>354</v>
       </c>
+      <c r="C101">
+        <v>0</v>
+      </c>
       <c r="F101" s="3">
         <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="G101" s="3">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="H101" s="3" t="e">
         <f t="shared" si="43"/>
@@ -11336,12 +11467,15 @@
       <c r="B102" t="s">
         <v>355</v>
       </c>
+      <c r="C102">
+        <v>0</v>
+      </c>
       <c r="F102" s="3">
         <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="G102" s="3">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="H102" s="3" t="e">
         <f t="shared" si="43"/>
@@ -11412,12 +11546,15 @@
       <c r="B103" t="s">
         <v>356</v>
       </c>
+      <c r="C103">
+        <v>0</v>
+      </c>
       <c r="F103" s="3">
         <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="G103" s="3">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="H103" s="3" t="e">
         <f t="shared" si="43"/>
@@ -11488,12 +11625,15 @@
       <c r="B104" t="s">
         <v>357</v>
       </c>
+      <c r="C104">
+        <v>0</v>
+      </c>
       <c r="F104" s="3">
         <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="G104" s="3">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="H104" s="3" t="e">
         <f t="shared" si="43"/>
@@ -11564,12 +11704,15 @@
       <c r="B105" t="s">
         <v>358</v>
       </c>
+      <c r="C105">
+        <v>0</v>
+      </c>
       <c r="F105" s="3">
         <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="G105" s="3">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="H105" s="3" t="e">
         <f t="shared" si="43"/>
@@ -11640,12 +11783,15 @@
       <c r="B106" t="s">
         <v>359</v>
       </c>
+      <c r="C106">
+        <v>0</v>
+      </c>
       <c r="F106" s="3">
         <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="G106" s="3">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="H106" s="3" t="e">
         <f t="shared" si="43"/>
@@ -11716,12 +11862,15 @@
       <c r="B107" t="s">
         <v>360</v>
       </c>
+      <c r="C107">
+        <v>0</v>
+      </c>
       <c r="F107" s="3">
         <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="G107" s="3">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="H107" s="3" t="e">
         <f t="shared" si="43"/>
@@ -11792,12 +11941,15 @@
       <c r="B108" t="s">
         <v>361</v>
       </c>
+      <c r="C108">
+        <v>0</v>
+      </c>
       <c r="F108" s="3">
         <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="G108" s="3">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="H108" s="3" t="e">
         <f t="shared" si="43"/>
@@ -11868,12 +12020,15 @@
       <c r="B109" t="s">
         <v>362</v>
       </c>
+      <c r="C109">
+        <v>0</v>
+      </c>
       <c r="F109" s="3">
         <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="G109" s="3">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="H109" s="3" t="e">
         <f t="shared" si="43"/>
@@ -11944,12 +12099,15 @@
       <c r="B110" t="s">
         <v>363</v>
       </c>
+      <c r="C110">
+        <v>0</v>
+      </c>
       <c r="F110" s="3">
         <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="G110" s="3">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="H110" s="3" t="e">
         <f t="shared" si="43"/>
@@ -12020,12 +12178,15 @@
       <c r="B111" t="s">
         <v>364</v>
       </c>
+      <c r="C111">
+        <v>0</v>
+      </c>
       <c r="F111" s="3">
         <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="G111" s="3">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="H111" s="3" t="e">
         <f t="shared" si="43"/>
@@ -12096,12 +12257,15 @@
       <c r="B112" t="s">
         <v>365</v>
       </c>
+      <c r="C112">
+        <v>0</v>
+      </c>
       <c r="F112" s="3">
         <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="G112" s="3">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="H112" s="3" t="e">
         <f t="shared" si="43"/>
@@ -12172,12 +12336,15 @@
       <c r="B113" t="s">
         <v>366</v>
       </c>
+      <c r="C113">
+        <v>0</v>
+      </c>
       <c r="F113" s="3">
         <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="G113" s="3">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="H113" s="3" t="e">
         <f t="shared" si="43"/>
@@ -12248,12 +12415,15 @@
       <c r="B114" t="s">
         <v>367</v>
       </c>
+      <c r="C114">
+        <v>0</v>
+      </c>
       <c r="F114" s="3">
         <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="G114" s="3">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="H114" s="3" t="e">
         <f t="shared" si="43"/>
@@ -12324,12 +12494,15 @@
       <c r="B115" t="s">
         <v>368</v>
       </c>
+      <c r="C115">
+        <v>0</v>
+      </c>
       <c r="F115" s="3">
         <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="G115" s="3">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="H115" s="3" t="e">
         <f t="shared" si="43"/>
@@ -12400,12 +12573,15 @@
       <c r="B116" t="s">
         <v>369</v>
       </c>
+      <c r="C116">
+        <v>0</v>
+      </c>
       <c r="F116" s="3">
         <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="G116" s="3">
-        <v>43</v>
+        <v>25</v>
       </c>
       <c r="H116" s="3" t="e">
         <f t="shared" si="43"/>
@@ -12469,103 +12645,593 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="117" spans="1:23" ht="16" x14ac:dyDescent="0.2">
-      <c r="A117" s="11"/>
-      <c r="B117" s="11"/>
-      <c r="F117" s="3"/>
-      <c r="G117" s="3"/>
-      <c r="H117" s="3"/>
-      <c r="I117" s="3"/>
-      <c r="J117" s="3"/>
-      <c r="K117" s="35"/>
-      <c r="O117" s="4"/>
-      <c r="P117" s="4"/>
-      <c r="Q117" s="4"/>
-      <c r="R117" s="4"/>
-    </row>
-    <row r="118" spans="1:23" ht="16" x14ac:dyDescent="0.2">
-      <c r="A118" s="11"/>
-      <c r="B118" s="11"/>
-      <c r="F118" s="3"/>
-      <c r="G118" s="3"/>
-      <c r="H118" s="3"/>
-      <c r="I118" s="3"/>
-      <c r="J118" s="3"/>
-      <c r="K118" s="35"/>
-      <c r="O118" s="4"/>
-      <c r="P118" s="4"/>
-      <c r="Q118" s="4"/>
-      <c r="R118" s="4"/>
-    </row>
-    <row r="119" spans="1:23" ht="16" x14ac:dyDescent="0.2">
-      <c r="A119" s="11"/>
-      <c r="B119" s="11"/>
-      <c r="F119" s="3"/>
-      <c r="G119" s="3"/>
-      <c r="H119" s="3"/>
-      <c r="I119" s="3"/>
-      <c r="J119" s="3"/>
-      <c r="K119" s="35"/>
-      <c r="O119" s="4"/>
-      <c r="P119" s="4"/>
-      <c r="Q119" s="4"/>
-      <c r="R119" s="4"/>
-    </row>
-    <row r="120" spans="1:23" ht="16" x14ac:dyDescent="0.2">
-      <c r="A120" s="11"/>
-      <c r="B120" s="11"/>
-      <c r="F120" s="3"/>
-      <c r="G120" s="3"/>
-      <c r="H120" s="3"/>
-      <c r="I120" s="3"/>
-      <c r="J120" s="3"/>
-      <c r="K120" s="35"/>
-      <c r="O120" s="4"/>
-      <c r="P120" s="4"/>
-      <c r="Q120" s="4"/>
-      <c r="R120" s="4"/>
-    </row>
-    <row r="121" spans="1:23" ht="16" x14ac:dyDescent="0.2">
-      <c r="A121" s="11"/>
-      <c r="B121" s="11"/>
-      <c r="F121" s="3"/>
-      <c r="G121" s="3"/>
-      <c r="H121" s="3"/>
-      <c r="I121" s="3"/>
-      <c r="J121" s="3"/>
-      <c r="K121" s="35"/>
-      <c r="O121" s="4"/>
-      <c r="P121" s="4"/>
-      <c r="Q121" s="4"/>
-      <c r="R121" s="4"/>
-    </row>
-    <row r="122" spans="1:23" ht="16" x14ac:dyDescent="0.2">
-      <c r="A122" s="11"/>
-      <c r="B122" s="11"/>
-      <c r="F122" s="3"/>
-      <c r="G122" s="3"/>
-      <c r="H122" s="3"/>
-      <c r="I122" s="3"/>
-      <c r="J122" s="3"/>
-      <c r="K122" s="35"/>
-      <c r="O122" s="4"/>
-      <c r="P122" s="4"/>
-      <c r="Q122" s="4"/>
-      <c r="R122" s="4"/>
-    </row>
-    <row r="123" spans="1:23" ht="16" x14ac:dyDescent="0.2">
-      <c r="A123" s="11"/>
-      <c r="B123" s="11"/>
-      <c r="F123" s="3"/>
-      <c r="G123" s="3"/>
-      <c r="H123" s="3"/>
-      <c r="I123" s="3"/>
-      <c r="J123" s="3"/>
-      <c r="K123" s="35"/>
-      <c r="O123" s="4"/>
-      <c r="P123" s="4"/>
-      <c r="Q123" s="4"/>
-      <c r="R123" s="4"/>
+    <row r="117" spans="1:23" s="41" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A117" s="48" t="s">
+        <v>372</v>
+      </c>
+      <c r="B117" s="48"/>
+      <c r="C117" s="41">
+        <v>18</v>
+      </c>
+      <c r="D117" s="41">
+        <v>6</v>
+      </c>
+      <c r="E117" s="41">
+        <v>1</v>
+      </c>
+      <c r="F117" s="49">
+        <f t="shared" si="42"/>
+        <v>0.108</v>
+      </c>
+      <c r="G117" s="49">
+        <v>25</v>
+      </c>
+      <c r="H117" s="49">
+        <f t="shared" si="43"/>
+        <v>231.48148148148147</v>
+      </c>
+      <c r="I117" s="49">
+        <f t="shared" si="44"/>
+        <v>64.8</v>
+      </c>
+      <c r="J117" s="49">
+        <f t="shared" si="45"/>
+        <v>48.6</v>
+      </c>
+      <c r="K117" s="49">
+        <f t="shared" si="46"/>
+        <v>108</v>
+      </c>
+      <c r="L117" s="41">
+        <f t="shared" si="47"/>
+        <v>4.8600000000000004E-2</v>
+      </c>
+      <c r="M117" s="50">
+        <v>25</v>
+      </c>
+      <c r="N117" s="51">
+        <v>0.45</v>
+      </c>
+      <c r="O117" s="52">
+        <f>(M117*N117)*1000/J117</f>
+        <v>231.48148148148147</v>
+      </c>
+      <c r="P117" s="52">
+        <f t="shared" ref="P117" si="48">N117*1000-O117</f>
+        <v>218.51851851851853</v>
+      </c>
+      <c r="Q117" s="53">
+        <f t="shared" ref="Q117" si="49">O117*0.7921/1000</f>
+        <v>0.18335648148148145</v>
+      </c>
+      <c r="R117" s="53">
+        <f t="shared" ref="R117" si="50">P117*0.7921</f>
+        <v>173.08851851851853</v>
+      </c>
+      <c r="S117" s="41">
+        <f>'print me lab dilution sheet'!H150</f>
+        <v>0</v>
+      </c>
+      <c r="T117" s="41">
+        <f>'print me lab dilution sheet'!I150</f>
+        <v>0</v>
+      </c>
+      <c r="U117" s="41">
+        <f t="shared" ref="U117" si="51">(S117/0.792)*1000</f>
+        <v>0</v>
+      </c>
+      <c r="V117" s="41">
+        <f t="shared" ref="V117" si="52">(T117/0.792)*1000</f>
+        <v>0</v>
+      </c>
+      <c r="W117" s="54" t="e">
+        <f t="shared" ref="W117" si="53">((U117*I117)/(U117+V117))</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="118" spans="1:23" s="41" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A118" s="48" t="s">
+        <v>373</v>
+      </c>
+      <c r="B118" s="48"/>
+      <c r="C118" s="41">
+        <v>13.4</v>
+      </c>
+      <c r="D118" s="41">
+        <v>6</v>
+      </c>
+      <c r="E118" s="41">
+        <v>1</v>
+      </c>
+      <c r="F118" s="49">
+        <f t="shared" ref="F118:F122" si="54">C118*D118/1000</f>
+        <v>8.0399999999999999E-2</v>
+      </c>
+      <c r="G118" s="49">
+        <v>25</v>
+      </c>
+      <c r="H118" s="49">
+        <f t="shared" ref="H118:H122" si="55">1/(F118/G118)</f>
+        <v>310.94527363184079</v>
+      </c>
+      <c r="I118" s="49">
+        <f t="shared" ref="I118:I122" si="56">(C118*D118/E118)*0.6</f>
+        <v>48.24</v>
+      </c>
+      <c r="J118" s="49">
+        <f t="shared" ref="J118:J122" si="57">(C118*D118/E118)*0.45</f>
+        <v>36.180000000000007</v>
+      </c>
+      <c r="K118" s="49">
+        <f t="shared" ref="K118:K122" si="58">(C118*D118/E118)</f>
+        <v>80.400000000000006</v>
+      </c>
+      <c r="L118" s="41">
+        <f t="shared" ref="L118:L122" si="59">J118*E118/1000</f>
+        <v>3.6180000000000004E-2</v>
+      </c>
+      <c r="M118" s="50">
+        <v>25</v>
+      </c>
+      <c r="N118" s="51">
+        <v>0.45</v>
+      </c>
+      <c r="O118" s="52">
+        <f>(M118*N118)*1000/J118</f>
+        <v>310.94527363184073</v>
+      </c>
+      <c r="P118" s="52">
+        <f t="shared" ref="P118:P122" si="60">N118*1000-O118</f>
+        <v>139.05472636815927</v>
+      </c>
+      <c r="Q118" s="53">
+        <f t="shared" ref="Q118:Q122" si="61">O118*0.7921/1000</f>
+        <v>0.24629975124378106</v>
+      </c>
+      <c r="R118" s="53">
+        <f t="shared" ref="R118:R122" si="62">P118*0.7921</f>
+        <v>110.14524875621896</v>
+      </c>
+      <c r="S118" s="41">
+        <f>'print me lab dilution sheet'!H151</f>
+        <v>0</v>
+      </c>
+      <c r="T118" s="41">
+        <f>'print me lab dilution sheet'!I151</f>
+        <v>0</v>
+      </c>
+      <c r="U118" s="41">
+        <f t="shared" ref="U118:U122" si="63">(S118/0.792)*1000</f>
+        <v>0</v>
+      </c>
+      <c r="V118" s="41">
+        <f t="shared" ref="V118:V122" si="64">(T118/0.792)*1000</f>
+        <v>0</v>
+      </c>
+      <c r="W118" s="54" t="e">
+        <f t="shared" ref="W118:W122" si="65">((U118*I118)/(U118+V118))</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="119" spans="1:23" s="41" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A119" s="48" t="s">
+        <v>374</v>
+      </c>
+      <c r="B119" s="48"/>
+      <c r="C119" s="41">
+        <v>6.19</v>
+      </c>
+      <c r="D119" s="41">
+        <v>6</v>
+      </c>
+      <c r="E119" s="41">
+        <v>1</v>
+      </c>
+      <c r="F119" s="49">
+        <f t="shared" si="54"/>
+        <v>3.7139999999999999E-2</v>
+      </c>
+      <c r="G119" s="49">
+        <v>25</v>
+      </c>
+      <c r="H119" s="49">
+        <f t="shared" si="55"/>
+        <v>673.12870220786215</v>
+      </c>
+      <c r="I119" s="49">
+        <f t="shared" si="56"/>
+        <v>22.283999999999999</v>
+      </c>
+      <c r="J119" s="49">
+        <f t="shared" si="57"/>
+        <v>16.713000000000001</v>
+      </c>
+      <c r="K119" s="49">
+        <f t="shared" si="58"/>
+        <v>37.14</v>
+      </c>
+      <c r="L119" s="41">
+        <f t="shared" si="59"/>
+        <v>1.6713000000000002E-2</v>
+      </c>
+      <c r="M119" s="50">
+        <v>25</v>
+      </c>
+      <c r="N119" s="51">
+        <v>0.45</v>
+      </c>
+      <c r="O119" s="52">
+        <f>(M119*N119)*1000/J119</f>
+        <v>673.12870220786215</v>
+      </c>
+      <c r="P119" s="52">
+        <f t="shared" si="60"/>
+        <v>-223.12870220786215</v>
+      </c>
+      <c r="Q119" s="53">
+        <f t="shared" si="61"/>
+        <v>0.53318524501884756</v>
+      </c>
+      <c r="R119" s="53">
+        <f t="shared" si="62"/>
+        <v>-176.74024501884762</v>
+      </c>
+      <c r="S119" s="41">
+        <f>'print me lab dilution sheet'!H152</f>
+        <v>0</v>
+      </c>
+      <c r="T119" s="41">
+        <f>'print me lab dilution sheet'!I152</f>
+        <v>0</v>
+      </c>
+      <c r="U119" s="41">
+        <f t="shared" si="63"/>
+        <v>0</v>
+      </c>
+      <c r="V119" s="41">
+        <f t="shared" si="64"/>
+        <v>0</v>
+      </c>
+      <c r="W119" s="54" t="e">
+        <f t="shared" si="65"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="120" spans="1:23" s="41" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A120" s="48" t="s">
+        <v>375</v>
+      </c>
+      <c r="B120" s="48"/>
+      <c r="C120" s="41">
+        <v>6.76</v>
+      </c>
+      <c r="D120" s="41">
+        <v>6</v>
+      </c>
+      <c r="E120" s="41">
+        <v>1</v>
+      </c>
+      <c r="F120" s="49">
+        <f t="shared" si="54"/>
+        <v>4.0559999999999999E-2</v>
+      </c>
+      <c r="G120" s="49">
+        <v>25</v>
+      </c>
+      <c r="H120" s="49">
+        <f t="shared" si="55"/>
+        <v>616.37080867850102</v>
+      </c>
+      <c r="I120" s="49">
+        <f t="shared" si="56"/>
+        <v>24.336000000000002</v>
+      </c>
+      <c r="J120" s="49">
+        <f t="shared" si="57"/>
+        <v>18.252000000000002</v>
+      </c>
+      <c r="K120" s="49">
+        <f t="shared" si="58"/>
+        <v>40.56</v>
+      </c>
+      <c r="L120" s="41">
+        <f t="shared" si="59"/>
+        <v>1.8252000000000001E-2</v>
+      </c>
+      <c r="M120" s="50">
+        <v>25</v>
+      </c>
+      <c r="N120" s="51">
+        <v>0.45</v>
+      </c>
+      <c r="O120" s="52">
+        <f>(M120*N120)*1000/J120</f>
+        <v>616.37080867850091</v>
+      </c>
+      <c r="P120" s="52">
+        <f t="shared" si="60"/>
+        <v>-166.37080867850091</v>
+      </c>
+      <c r="Q120" s="53">
+        <f t="shared" si="61"/>
+        <v>0.48822731755424059</v>
+      </c>
+      <c r="R120" s="53">
+        <f t="shared" si="62"/>
+        <v>-131.78231755424056</v>
+      </c>
+      <c r="S120" s="41">
+        <f>'print me lab dilution sheet'!H153</f>
+        <v>0</v>
+      </c>
+      <c r="T120" s="41">
+        <f>'print me lab dilution sheet'!I153</f>
+        <v>0</v>
+      </c>
+      <c r="U120" s="41">
+        <f t="shared" si="63"/>
+        <v>0</v>
+      </c>
+      <c r="V120" s="41">
+        <f t="shared" si="64"/>
+        <v>0</v>
+      </c>
+      <c r="W120" s="54" t="e">
+        <f t="shared" si="65"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="121" spans="1:23" s="41" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A121" s="48" t="s">
+        <v>376</v>
+      </c>
+      <c r="B121" s="48"/>
+      <c r="C121" s="41">
+        <v>4.09</v>
+      </c>
+      <c r="D121" s="41">
+        <v>6</v>
+      </c>
+      <c r="E121" s="41">
+        <v>1</v>
+      </c>
+      <c r="F121" s="49">
+        <f t="shared" si="54"/>
+        <v>2.4539999999999999E-2</v>
+      </c>
+      <c r="G121" s="49">
+        <v>25</v>
+      </c>
+      <c r="H121" s="49">
+        <f t="shared" si="55"/>
+        <v>1018.7449062754686</v>
+      </c>
+      <c r="I121" s="49">
+        <f t="shared" si="56"/>
+        <v>14.723999999999998</v>
+      </c>
+      <c r="J121" s="49">
+        <f t="shared" si="57"/>
+        <v>11.042999999999999</v>
+      </c>
+      <c r="K121" s="49">
+        <f t="shared" si="58"/>
+        <v>24.54</v>
+      </c>
+      <c r="L121" s="41">
+        <f t="shared" si="59"/>
+        <v>1.1042999999999999E-2</v>
+      </c>
+      <c r="M121" s="50">
+        <v>25</v>
+      </c>
+      <c r="N121" s="51">
+        <v>0.45</v>
+      </c>
+      <c r="O121" s="52">
+        <f>(M121*N121)*1000/J121</f>
+        <v>1018.7449062754687</v>
+      </c>
+      <c r="P121" s="52">
+        <f t="shared" si="60"/>
+        <v>-568.74490627546868</v>
+      </c>
+      <c r="Q121" s="53">
+        <f t="shared" si="61"/>
+        <v>0.8069478402607988</v>
+      </c>
+      <c r="R121" s="53">
+        <f t="shared" si="62"/>
+        <v>-450.50284026079873</v>
+      </c>
+      <c r="S121" s="41">
+        <f>'print me lab dilution sheet'!H154</f>
+        <v>0</v>
+      </c>
+      <c r="T121" s="41">
+        <f>'print me lab dilution sheet'!I154</f>
+        <v>0</v>
+      </c>
+      <c r="U121" s="41">
+        <f t="shared" si="63"/>
+        <v>0</v>
+      </c>
+      <c r="V121" s="41">
+        <f t="shared" si="64"/>
+        <v>0</v>
+      </c>
+      <c r="W121" s="54" t="e">
+        <f t="shared" si="65"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="122" spans="1:23" s="41" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A122" s="48" t="s">
+        <v>377</v>
+      </c>
+      <c r="B122" s="48"/>
+      <c r="C122" s="41">
+        <v>11.28</v>
+      </c>
+      <c r="D122" s="41">
+        <v>6</v>
+      </c>
+      <c r="E122" s="41">
+        <v>1</v>
+      </c>
+      <c r="F122" s="49">
+        <f t="shared" si="54"/>
+        <v>6.767999999999999E-2</v>
+      </c>
+      <c r="G122" s="49">
+        <v>25</v>
+      </c>
+      <c r="H122" s="49">
+        <f t="shared" si="55"/>
+        <v>369.38534278959816</v>
+      </c>
+      <c r="I122" s="49">
+        <f t="shared" si="56"/>
+        <v>40.607999999999997</v>
+      </c>
+      <c r="J122" s="49">
+        <f t="shared" si="57"/>
+        <v>30.455999999999996</v>
+      </c>
+      <c r="K122" s="49">
+        <f t="shared" si="58"/>
+        <v>67.679999999999993</v>
+      </c>
+      <c r="L122" s="41">
+        <f t="shared" si="59"/>
+        <v>3.0455999999999997E-2</v>
+      </c>
+      <c r="M122" s="50">
+        <v>25</v>
+      </c>
+      <c r="N122" s="51">
+        <v>0.45</v>
+      </c>
+      <c r="O122" s="52">
+        <f>(M122*N122)*1000/J122</f>
+        <v>369.38534278959816</v>
+      </c>
+      <c r="P122" s="52">
+        <f t="shared" si="60"/>
+        <v>80.614657210401845</v>
+      </c>
+      <c r="Q122" s="53">
+        <f t="shared" si="61"/>
+        <v>0.2925901300236407</v>
+      </c>
+      <c r="R122" s="53">
+        <f t="shared" si="62"/>
+        <v>63.854869976359304</v>
+      </c>
+      <c r="S122" s="41">
+        <f>'print me lab dilution sheet'!H155</f>
+        <v>0</v>
+      </c>
+      <c r="T122" s="41">
+        <f>'print me lab dilution sheet'!I155</f>
+        <v>0</v>
+      </c>
+      <c r="U122" s="41">
+        <f t="shared" si="63"/>
+        <v>0</v>
+      </c>
+      <c r="V122" s="41">
+        <f t="shared" si="64"/>
+        <v>0</v>
+      </c>
+      <c r="W122" s="54" t="e">
+        <f t="shared" si="65"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="123" spans="1:23" s="41" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A123" s="48" t="s">
+        <v>378</v>
+      </c>
+      <c r="B123" s="48"/>
+      <c r="C123" s="41">
+        <v>26.14</v>
+      </c>
+      <c r="D123" s="41">
+        <v>6</v>
+      </c>
+      <c r="E123" s="41">
+        <v>1</v>
+      </c>
+      <c r="F123" s="49">
+        <f t="shared" ref="F123" si="66">C123*D123/1000</f>
+        <v>0.15684000000000001</v>
+      </c>
+      <c r="G123" s="49">
+        <v>25</v>
+      </c>
+      <c r="H123" s="49">
+        <f t="shared" ref="H123" si="67">1/(F123/G123)</f>
+        <v>159.39811272634529</v>
+      </c>
+      <c r="I123" s="49">
+        <f t="shared" ref="I123" si="68">(C123*D123/E123)*0.6</f>
+        <v>94.103999999999999</v>
+      </c>
+      <c r="J123" s="49">
+        <f t="shared" ref="J123" si="69">(C123*D123/E123)*0.45</f>
+        <v>70.578000000000003</v>
+      </c>
+      <c r="K123" s="49">
+        <f t="shared" ref="K123" si="70">(C123*D123/E123)</f>
+        <v>156.84</v>
+      </c>
+      <c r="L123" s="41">
+        <f t="shared" ref="L123" si="71">J123*E123/1000</f>
+        <v>7.0578000000000002E-2</v>
+      </c>
+      <c r="M123" s="50">
+        <v>25</v>
+      </c>
+      <c r="N123" s="51">
+        <v>0.45</v>
+      </c>
+      <c r="O123" s="52">
+        <f>(M123*N123)*1000/J123</f>
+        <v>159.39811272634532</v>
+      </c>
+      <c r="P123" s="52">
+        <f t="shared" ref="P123" si="72">N123*1000-O123</f>
+        <v>290.60188727365471</v>
+      </c>
+      <c r="Q123" s="53">
+        <f t="shared" ref="Q123" si="73">O123*0.7921/1000</f>
+        <v>0.12625924509053812</v>
+      </c>
+      <c r="R123" s="53">
+        <f t="shared" ref="R123" si="74">P123*0.7921</f>
+        <v>230.18575490946191</v>
+      </c>
+      <c r="S123" s="41">
+        <f>'print me lab dilution sheet'!H156</f>
+        <v>0</v>
+      </c>
+      <c r="T123" s="41">
+        <f>'print me lab dilution sheet'!I156</f>
+        <v>0</v>
+      </c>
+      <c r="U123" s="41">
+        <f t="shared" ref="U123" si="75">(S123/0.792)*1000</f>
+        <v>0</v>
+      </c>
+      <c r="V123" s="41">
+        <f t="shared" ref="V123" si="76">(T123/0.792)*1000</f>
+        <v>0</v>
+      </c>
+      <c r="W123" s="54" t="e">
+        <f t="shared" ref="W123" si="77">((U123*I123)/(U123+V123))</f>
+        <v>#DIV/0!</v>
+      </c>
     </row>
     <row r="124" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A124" s="11"/>
@@ -16823,7 +17489,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DA53AE6-5E23-2442-8563-4CA30FF6662F}">
   <dimension ref="A1:I210"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A114" sqref="A114:A139"/>
     </sheetView>
   </sheetViews>
@@ -21312,12 +21978,14 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="5cece13e-3376-4417-9525-be60b11a89a8" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="03570766-e33a-4164-8943-6d32a7ac417a">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -21549,20 +22217,28 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="5cece13e-3376-4417-9525-be60b11a89a8" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="03570766-e33a-4164-8943-6d32a7ac417a">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DB7F15B3-A81F-4A71-B0B7-DFC0AD11F1D1}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FF21F518-5840-4B9C-B7A7-C68FEFA76CF1}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="482683a9-e61d-4853-b10b-3f4a908e17aa"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="5cece13e-3376-4417-9525-be60b11a89a8"/>
+    <ds:schemaRef ds:uri="03570766-e33a-4164-8943-6d32a7ac417a"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -21588,19 +22264,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FF21F518-5840-4B9C-B7A7-C68FEFA76CF1}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DB7F15B3-A81F-4A71-B0B7-DFC0AD11F1D1}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="482683a9-e61d-4853-b10b-3f4a908e17aa"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="5cece13e-3376-4417-9525-be60b11a89a8"/>
-    <ds:schemaRef ds:uri="03570766-e33a-4164-8943-6d32a7ac417a"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>